<commit_message>
parsing for GWAS Catalog
</commit_message>
<xml_diff>
--- a/meta/megastroke/megastroke.apoe.xlsx
+++ b/meta/megastroke/megastroke.apoe.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slaan3/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slaan3/git/CirculatoryHealth/AAO_IschemicStroke/meta/megastroke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D64DC82-E719-4F40-AB4E-51FB217C96A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45606583-CDAD-0D4B-BEB3-9EE55003CAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{BFF4B0EC-0482-CA43-AD37-125BC5CB4FE0}"/>
+    <workbookView xWindow="760" yWindow="9260" windowWidth="28040" windowHeight="17440" xr2:uid="{BFF4B0EC-0482-CA43-AD37-125BC5CB4FE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>MarkerName</t>
   </si>
@@ -161,14 +162,113 @@
   </si>
   <si>
     <t>----??</t>
+  </si>
+  <si>
+    <t>-+--+----+++-+-</t>
+  </si>
+  <si>
+    <t>Phenotype</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>with SiGN</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>IS_EUR.GC_1.txt.gz</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>ALLSTROKE_EUR.GC_1.txt.gz</t>
+  </si>
+  <si>
+    <t>--+--+----+++-+-</t>
+  </si>
+  <si>
+    <t>CE_EUR.GC_1.txt.gz</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>CES</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>LAS</t>
+  </si>
+  <si>
+    <t>SVS</t>
+  </si>
+  <si>
+    <t>+++-+--+?+-+</t>
+  </si>
+  <si>
+    <t>+--+++---</t>
+  </si>
+  <si>
+    <t>LAS_EUR.GC_1.txt.gz</t>
+  </si>
+  <si>
+    <t>SVD_EUR.GC_1.txt.gz</t>
+  </si>
+  <si>
+    <t>-?+-+--+++-</t>
+  </si>
+  <si>
+    <t>EAF</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>Allele2_EffectAllele</t>
+  </si>
+  <si>
+    <t>Allele1_OtherAllele</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -193,13 +293,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -216,9 +323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -362,7 +469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,7 +611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,13 +619,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EE012B-56AF-5E47-A3EB-CAF03E7A7C31}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="K8" sqref="K8:U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -803,6 +915,429 @@
       </c>
       <c r="AE3">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8">
+        <v>0.8488</v>
+      </c>
+      <c r="H8">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>-0.02</v>
+      </c>
+      <c r="J8">
+        <v>1.47E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <f>1-G8</f>
+        <v>0.1512</v>
+      </c>
+      <c r="L8" s="2">
+        <f>-I8</f>
+        <v>0.02</v>
+      </c>
+      <c r="M8" s="3">
+        <f>J8</f>
+        <v>1.47E-2</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.17530000000000001</v>
+      </c>
+      <c r="O8" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" s="5">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>24.695</v>
+      </c>
+      <c r="R8">
+        <v>15</v>
+      </c>
+      <c r="S8" s="3">
+        <v>5.4190000000000002E-2</v>
+      </c>
+      <c r="T8" s="4">
+        <v>414547</v>
+      </c>
+      <c r="U8" s="4">
+        <v>32475</v>
+      </c>
+      <c r="V8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <v>0.84919999999999995</v>
+      </c>
+      <c r="H9">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="I9">
+        <v>-4.7999999999999996E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <f>1-G9</f>
+        <v>0.15080000000000005</v>
+      </c>
+      <c r="L9" s="2">
+        <f>-I9</f>
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="M9" s="3">
+        <f>J9</f>
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.76890000000000003</v>
+      </c>
+      <c r="O9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="5">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>21.305</v>
+      </c>
+      <c r="R9">
+        <v>14</v>
+      </c>
+      <c r="S9" s="3">
+        <v>9.4070000000000001E-2</v>
+      </c>
+      <c r="T9" s="4">
+        <v>399337</v>
+      </c>
+      <c r="U9" s="4">
+        <v>26193</v>
+      </c>
+      <c r="V9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <v>0.84740000000000004</v>
+      </c>
+      <c r="H10">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="J10">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ref="K10:K12" si="0">1-G10</f>
+        <v>0.15259999999999996</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" ref="L10:L12" si="1">-I10</f>
+        <v>-3.1300000000000001E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" ref="M10:M12" si="2">J10</f>
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.34710000000000002</v>
+      </c>
+      <c r="O10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>8.36</v>
+      </c>
+      <c r="R10">
+        <v>10</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.59370000000000001</v>
+      </c>
+      <c r="T10" s="4">
+        <v>289083</v>
+      </c>
+      <c r="U10" s="4">
+        <v>4908</v>
+      </c>
+      <c r="V10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <v>0.85189999999999999</v>
+      </c>
+      <c r="H11">
+        <v>1.89E-2</v>
+      </c>
+      <c r="I11">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="J11">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14810000000000001</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.2000000000000002E-3</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="2"/>
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.93989999999999996</v>
+      </c>
+      <c r="O11" t="s">
+        <v>59</v>
+      </c>
+      <c r="P11" s="5">
+        <v>41.4</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>13.648</v>
+      </c>
+      <c r="R11">
+        <v>8</v>
+      </c>
+      <c r="S11" s="3">
+        <v>9.1410000000000005E-2</v>
+      </c>
+      <c r="T11" s="4">
+        <v>185768</v>
+      </c>
+      <c r="U11" s="4">
+        <v>3120</v>
+      </c>
+      <c r="V11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="H12">
+        <v>1.43E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="J12">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.15269999999999995</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.6500000000000001E-2</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="2"/>
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.67869999999999997</v>
+      </c>
+      <c r="O12" t="s">
+        <v>62</v>
+      </c>
+      <c r="P12" s="5">
+        <v>6.1</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>9.5850000000000009</v>
+      </c>
+      <c r="R12">
+        <v>9</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0.3851</v>
+      </c>
+      <c r="T12" s="4">
+        <v>225764</v>
+      </c>
+      <c r="U12" s="4">
+        <v>3821</v>
+      </c>
+      <c r="V12" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>